<commit_message>
my second booob girl
</commit_message>
<xml_diff>
--- a/call statistics2.xlsx
+++ b/call statistics2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Muna Moses\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Muna Moses\Desktop\new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A06D850-498C-4FCE-A9B5-2E7935AC48AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743337C5-F0D1-4055-A420-BE46E82021D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{1DA04E72-C5F5-45B4-90D8-8E39D6BDF85E}"/>
   </bookViews>
@@ -30,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -217,9 +216,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -411,20 +410,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -441,20 +433,42 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -462,27 +476,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -810,178 +808,178 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="34">
         <v>40544</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="11">
         <v>7.5</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="11">
         <v>35</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="12">
         <f>C4*D4</f>
         <v>262.5</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="12">
         <f>E4*0.06</f>
         <v>15.75</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="12">
         <f>E4-F4</f>
         <v>246.75</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="11">
         <v>8</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="11">
         <v>30</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="12">
         <f t="shared" ref="E5:E8" si="0">C5*D5</f>
         <v>240</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="12">
         <f t="shared" ref="F5:F8" si="1">E5*0.06</f>
         <v>14.399999999999999</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="12">
         <f t="shared" ref="G5:G8" si="2">E5-F5</f>
         <v>225.6</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="11">
         <v>6.5</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="11">
         <v>25</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="12">
         <f t="shared" si="0"/>
         <v>162.5</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="12">
         <f t="shared" si="1"/>
         <v>9.75</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="12">
         <f t="shared" si="2"/>
         <v>152.75</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="11">
         <v>9</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="11">
         <v>40</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="12">
         <f t="shared" si="0"/>
         <v>360</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="12">
         <f t="shared" si="1"/>
         <v>21.599999999999998</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="12">
         <f t="shared" si="2"/>
         <v>338.4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="11">
         <v>10</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="11">
         <v>39</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="12">
         <f t="shared" si="0"/>
         <v>390</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="12">
         <f t="shared" si="1"/>
         <v>23.4</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="12">
         <f t="shared" si="2"/>
         <v>366.6</v>
       </c>
@@ -1012,190 +1010,180 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7"/>
+      <c r="A2" s="3"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="11">
         <v>42</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="11">
         <v>5</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="11">
         <f>B4/C4</f>
         <v>8.4</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="25">
         <f>D4*B12</f>
         <v>2.1</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="11">
         <v>6</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="11">
         <v>4</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="11">
         <f t="shared" ref="D5:D8" si="0">B5/C5</f>
         <v>1.5</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="25">
         <f t="shared" ref="E5:E8" si="1">D5*B13</f>
         <v>0</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="11">
         <v>39</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="11">
         <v>6</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="11">
         <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="11">
         <v>15</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="11">
         <v>6</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="11">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="11">
         <v>2</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="11">
         <v>7</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="28">
         <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="7"/>
+      <c r="A9" s="3"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="17">
         <f>SUM(B4:B8)</f>
         <v>104</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="17">
         <f t="shared" ref="C10:E10" si="2">SUM(C4:C8)</f>
         <v>28</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="29">
         <f t="shared" si="2"/>
         <v>19.185714285714283</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="17">
         <f t="shared" si="2"/>
         <v>2.1</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="7"/>
+      <c r="A11" s="3"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="15">
         <v>0.25</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="9"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1210,7 +1198,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,299 +1211,304 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="37"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="30"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="32" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="31">
         <v>1600</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="31">
         <v>2500</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="31">
         <f>D5*0.02</f>
         <v>50</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="31">
         <f>C5+E5</f>
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="31">
         <v>1800</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="31">
         <v>3000</v>
       </c>
-      <c r="E6" s="38">
-        <f t="shared" ref="E6:E10" si="0">D6*0.02</f>
+      <c r="E6" s="31">
+        <f t="shared" ref="E6:E11" si="0">D6*0.02</f>
         <v>60</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6" s="31">
         <f t="shared" ref="F6:F10" si="1">C6+E6</f>
         <v>1860</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="31">
         <v>1500</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="31">
         <v>2200</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="31">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="31">
         <f t="shared" si="1"/>
         <v>1544</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="31">
         <v>2000</v>
       </c>
-      <c r="D8" s="38">
+      <c r="D8" s="31">
         <v>4500</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="31">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="F8" s="38">
+      <c r="F8" s="31">
         <f t="shared" si="1"/>
         <v>2090</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="31">
         <v>1700</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="31">
         <v>3500</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9" s="31">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="F9" s="38">
+      <c r="F9" s="31">
         <f t="shared" si="1"/>
         <v>1770</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="31">
         <v>1600</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="31">
         <v>2500</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="31">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="31">
         <f t="shared" si="1"/>
         <v>1650</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31">
+        <v>100000000</v>
+      </c>
+      <c r="E11" s="31">
+        <f t="shared" si="0"/>
+        <v>2000000</v>
+      </c>
+      <c r="F11" s="31"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="17" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="38">
+      <c r="C12" s="31">
         <f>SUM(C5:C10)</f>
         <v>10200</v>
       </c>
-      <c r="D12" s="38">
-        <f t="shared" ref="D12:F12" si="2">SUM(D5:D10)</f>
-        <v>18200</v>
-      </c>
-      <c r="E12" s="38">
-        <f t="shared" si="2"/>
-        <v>364</v>
-      </c>
-      <c r="F12" s="38">
-        <f t="shared" si="2"/>
+      <c r="D12" s="31">
+        <f>SUM(D5:D11)</f>
+        <v>100018200</v>
+      </c>
+      <c r="E12" s="31">
+        <f>SUM(E5:E11)</f>
+        <v>2000364</v>
+      </c>
+      <c r="F12" s="31">
+        <f t="shared" ref="D12:F12" si="2">SUM(F5:F10)</f>
         <v>10564</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="17" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="38">
+      <c r="C13" s="31">
         <f>AVERAGE(C5:C10)</f>
         <v>1700</v>
       </c>
-      <c r="D13" s="38">
-        <f t="shared" ref="D13:F13" si="3">AVERAGE(D5:D10)</f>
-        <v>3033.3333333333335</v>
-      </c>
-      <c r="E13" s="38">
-        <f t="shared" si="3"/>
-        <v>60.666666666666664</v>
-      </c>
-      <c r="F13" s="38">
-        <f t="shared" si="3"/>
+      <c r="D13" s="31">
+        <f>AVERAGE(D5:D11)</f>
+        <v>14288314.285714285</v>
+      </c>
+      <c r="E13" s="31">
+        <f>AVERAGE(E5:E11)</f>
+        <v>285766.28571428574</v>
+      </c>
+      <c r="F13" s="31">
+        <f t="shared" ref="D13:F13" si="3">AVERAGE(F5:F10)</f>
         <v>1760.6666666666667</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="17" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="38">
+      <c r="C14" s="31">
         <f>LARGE(C5:C10,1)</f>
         <v>2000</v>
       </c>
-      <c r="D14" s="38">
+      <c r="D14" s="31">
         <f t="shared" ref="D14:F14" si="4">LARGE(D5:D10,1)</f>
         <v>4500</v>
       </c>
-      <c r="E14" s="38">
+      <c r="E14" s="31">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
-      <c r="F14" s="38">
+      <c r="F14" s="31">
         <f t="shared" si="4"/>
         <v>2090</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="17" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="38">
+      <c r="C15" s="31">
         <f>SMALL(C5:C10,1)</f>
         <v>1500</v>
       </c>
-      <c r="D15" s="38">
+      <c r="D15" s="31">
         <f t="shared" ref="D15:F15" si="5">SMALL(D5:D10,1)</f>
         <v>2200</v>
       </c>
-      <c r="E15" s="38">
+      <c r="E15" s="31">
         <f t="shared" si="5"/>
         <v>44</v>
       </c>
-      <c r="F15" s="38">
+      <c r="F15" s="31">
         <f t="shared" si="5"/>
         <v>1544</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="17" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="38">
+      <c r="C16" s="31">
         <f>COUNT(C5:C10)</f>
         <v>6</v>
       </c>
-      <c r="D16" s="38">
+      <c r="D16" s="31">
         <f t="shared" ref="D16:F16" si="6">COUNT(D5:D10)</f>
         <v>6</v>
       </c>
-      <c r="E16" s="38">
+      <c r="E16" s="31">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="F16" s="38">
+      <c r="F16" s="31">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>

</xml_diff>